<commit_message>
Correção de tratamento de data
</commit_message>
<xml_diff>
--- a/Resultado.xlsx
+++ b/Resultado.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -624,7 +624,7 @@
         <v>44845</v>
       </c>
       <c r="W2" s="2" t="n">
-        <v>45572</v>
+        <v>45483</v>
       </c>
     </row>
     <row r="3">
@@ -701,7 +701,7 @@
         <v>45541</v>
       </c>
       <c r="W3" s="2" t="n">
-        <v>45542</v>
+        <v>45482</v>
       </c>
     </row>
     <row r="4">
@@ -788,47 +788,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>RODRIGO DOS SANTOS GENASIO</t>
+          <t>JOSE FELIX RODRIGUES NETO</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>373.813.358-59</t>
+          <t>218.805.223-49</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>11-95783-0792</t>
+          <t>11-99258-5964</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">rodrigogenasio2021@gmail.com </t>
+          <t xml:space="preserve">josefelix.neto54@gmail.com </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>SANDRA D´ ANGELO  MONTENEGRO</t>
+          <t>AZOR MARTIN GRILO</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>163.408.318-00</t>
+          <t>082.202.578-73</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>11-97503-4446</t>
+          <t>11 94498-7971</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>sdmontenegro@uol.com.br</t>
+          <t xml:space="preserve">azorgrilo@bol.com.br </t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Rua Basilio Marques, nº 7 - Centro</t>
+          <t>Rua Maria Giacco Ramos, 420 - César de Souza</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -836,16 +836,16 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>3.000,00</t>
+          <t>2.000,00</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>05/10/2023</t>
+          <t>03/08/2024</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
@@ -856,35 +856,33 @@
         </is>
       </c>
       <c r="T5" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U5" t="inlineStr"/>
       <c r="V5" s="2" t="n">
-        <v>45057</v>
-      </c>
-      <c r="W5" s="2" t="n">
-        <v>45419</v>
-      </c>
+        <v>45513</v>
+      </c>
+      <c r="W5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">MATSU REVESTIMENTOS EIRELI </t>
+          <t>RODRIGO DOS SANTOS GENASIO</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>32.489.204/0001-24</t>
+          <t>373.813.358-59</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11-97506-1669</t>
+          <t>11-95783-0792</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">nitchan_pescador@hotmail.com </t>
+          <t xml:space="preserve">rodrigogenasio2021@gmail.com </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -909,7 +907,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Rua Basilio Marques, nº 17 - Centro</t>
+          <t>Rua Basilio Marques, nº 7 - Centro</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -917,16 +915,16 @@
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>3.844,00</t>
+          <t>3.000,00</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>15/03/2023</t>
+          <t>05/10/2023</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
@@ -937,60 +935,60 @@
         </is>
       </c>
       <c r="T6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U6" t="inlineStr"/>
       <c r="V6" s="2" t="n">
-        <v>45015</v>
+        <v>45057</v>
       </c>
       <c r="W6" s="2" t="n">
-        <v>45503</v>
+        <v>45478</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>JOSÉ ROBERTO DE OLIVEIRA</t>
+          <t xml:space="preserve">MATSU REVESTIMENTOS EIRELI </t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>042.156.538-19</t>
+          <t>32.489.204/0001-24</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11-95444-1475</t>
+          <t>11-97506-1669</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">janefdc243@gmail.com </t>
+          <t xml:space="preserve">nitchan_pescador@hotmail.com </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>AZOR MARTIN GRILO</t>
+          <t>SANDRA D´ ANGELO  MONTENEGRO</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>082.202.578-73</t>
+          <t>163.408.318-00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>11 94498-7971</t>
+          <t>11-97503-4446</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t xml:space="preserve">azorgrilo@bol.com.br </t>
+          <t>sdmontenegro@uol.com.br</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Rua Nito sona, 1.235 - Jundiapeba</t>
+          <t>Rua Basilio Marques, nº 17 - Centro</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -998,16 +996,16 @@
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>1.000,00</t>
+          <t>3.844,00</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>30/11/2022</t>
+          <t>15/03/2023</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
@@ -1022,7 +1020,7 @@
       </c>
       <c r="U7" t="inlineStr"/>
       <c r="V7" s="2" t="n">
-        <v>45290</v>
+        <v>45015</v>
       </c>
       <c r="W7" s="2" t="n">
         <v>45503</v>
@@ -1031,47 +1029,47 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">CLODOALDO GUIMARÃES PIRES </t>
+          <t>JOSÉ ROBERTO DE OLIVEIRA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>01.543272/0001-09</t>
+          <t>042.156.538-19</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>11-96343-2158</t>
+          <t>11-95444-1475</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">clodoaldogp@hotmail.com </t>
+          <t xml:space="preserve">janefdc243@gmail.com </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>SANDRA D´ ANGELO  MONTENEGRO</t>
+          <t>AZOR MARTIN GRILO</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>163.408.318-00</t>
+          <t>082.202.578-73</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>11-97503-4446</t>
+          <t>11 94498-7971</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>sdmontenegro@uol.com.br</t>
+          <t xml:space="preserve">azorgrilo@bol.com.br </t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Rua Engenheiro Gualberto, 378 - Centro</t>
+          <t>Rua Nito sona, 1.235 - Jundiapeba</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -1079,16 +1077,16 @@
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr">
         <is>
-          <t>1.650,00</t>
+          <t>1.000,00</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>29/02/2020</t>
+          <t>30/11/2022</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
@@ -1103,56 +1101,56 @@
       </c>
       <c r="U8" t="inlineStr"/>
       <c r="V8" s="2" t="n">
-        <v>43955</v>
+        <v>45290</v>
       </c>
       <c r="W8" s="2" t="n">
-        <v>45419</v>
+        <v>45503</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>WILLIAN GABRIEL SILVA PINTO</t>
+          <t xml:space="preserve">CLODOALDO GUIMARÃES PIRES </t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>373.473.428-21</t>
+          <t>01.543272/0001-09</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>11-97597-5142</t>
+          <t>11-96343-2158</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">willianpalestra10@gmail.com </t>
+          <t xml:space="preserve">clodoaldogp@hotmail.com </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>AZOR MARTIN GRILO</t>
+          <t>SANDRA D´ ANGELO  MONTENEGRO</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>082.202.578-73</t>
+          <t>163.408.318-00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>11 94498-7971</t>
+          <t>11-97503-4446</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t xml:space="preserve">azorgrilo@bol.com.br </t>
+          <t>sdmontenegro@uol.com.br</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Av. Ezelino da Cunha Glória - Bloco 670 B - APTO 22</t>
+          <t>Rua Engenheiro Gualberto, 378 - Centro</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -1160,16 +1158,16 @@
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
-          <t>1.100,00</t>
+          <t>1.650,00</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>30/11/2023</t>
+          <t>29/02/2020</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
@@ -1184,56 +1182,56 @@
       </c>
       <c r="U9" t="inlineStr"/>
       <c r="V9" s="2" t="n">
-        <v>45474</v>
+        <v>43955</v>
       </c>
       <c r="W9" s="2" t="n">
-        <v>45480</v>
+        <v>45478</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>VIVIANE DINIZ QUINTÃO</t>
+          <t>WILLIAN GABRIEL SILVA PINTO</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>338.480.558-56</t>
+          <t>373.473.428-21</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>11-95939-1201</t>
+          <t>11-97597-5142</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">soleny.diniz023@gmail.com </t>
+          <t xml:space="preserve">willianpalestra10@gmail.com </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>WELLINGTON  GATTI MIYATAKE</t>
+          <t>AZOR MARTIN GRILO</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>342.236.248-73</t>
+          <t>082.202.578-73</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 80-6342-1902</t>
+          <t>11 94498-7971</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t xml:space="preserve">wellmiyatake@gmail.com </t>
+          <t xml:space="preserve">azorgrilo@bol.com.br </t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Av. Ezelino da Cunha Glória - Bloco 629 A - APTO 44</t>
+          <t>Av. Ezelino da Cunha Glória - Bloco 670 B - APTO 22</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
@@ -1246,7 +1244,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>02/02/2024</t>
+          <t>30/11/2023</t>
         </is>
       </c>
       <c r="O10" t="n">
@@ -1261,56 +1259,60 @@
         </is>
       </c>
       <c r="T10" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U10" t="inlineStr"/>
       <c r="V10" s="2" t="n">
-        <v>45538</v>
+        <v>45474</v>
       </c>
       <c r="W10" s="2" t="n">
-        <v>45542</v>
+        <v>45480</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>JOÃO VICTOR DA CUNHA BRANCO</t>
+          <t>VIVIANE DINIZ QUINTÃO</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>493.294.358-07</t>
+          <t>338.480.558-56</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>11-99181-4902</t>
+          <t>11-95939-1201</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">brunobranco658@gmail.com </t>
+          <t xml:space="preserve">soleny.diniz023@gmail.com </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ROGÉRIO CESÁRIO GRILLO</t>
+          <t>WELLINGTON  GATTI MIYATAKE</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>329.849.998-60</t>
+          <t>342.236.248-73</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>11 99549-5072</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
+          <t xml:space="preserve"> 80-6342-1902</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wellmiyatake@gmail.com </t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Rua João Benegas Ortiz - Bloco 925 A - Condomínio Topazio</t>
+          <t>Av. Ezelino da Cunha Glória - Bloco 629 A - APTO 44</t>
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
@@ -1323,7 +1325,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>23/01/2023</t>
+          <t>02/02/2024</t>
         </is>
       </c>
       <c r="O11" t="n">
@@ -1342,56 +1344,52 @@
       </c>
       <c r="U11" t="inlineStr"/>
       <c r="V11" s="2" t="n">
-        <v>44985</v>
+        <v>45538</v>
       </c>
       <c r="W11" s="2" t="n">
-        <v>45503</v>
+        <v>45482</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SABRINA FARIAS DE ALMEIDA</t>
+          <t>JOÃO VICTOR DA CUNHA BRANCO</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>395.792.568-10</t>
+          <t>493.294.358-07</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11-98938-5786</t>
+          <t>11-99181-4902</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">sabrinafarias22@hotmail.com </t>
+          <t xml:space="preserve">brunobranco658@gmail.com </t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>SANDRA D´ ANGELO  MONTENEGRO</t>
+          <t>ROGÉRIO CESÁRIO GRILLO</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>163.408.318-00</t>
+          <t>329.849.998-60</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>11-97503-4446</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>sdmontenegro@uol.com.br</t>
-        </is>
-      </c>
+          <t>11 99549-5072</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Rua Engenheiro Gualberto, 366 - Centro</t>
+          <t>Rua João Benegas Ortiz - Bloco 925 A - Condomínio Topazio</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
@@ -1399,16 +1397,16 @@
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
-          <t>854,00</t>
+          <t>1.100,00</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>12/01/2023</t>
+          <t>23/01/2023</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
@@ -1419,60 +1417,60 @@
         </is>
       </c>
       <c r="T12" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U12" t="inlineStr"/>
       <c r="V12" s="2" t="n">
-        <v>45262</v>
+        <v>44985</v>
       </c>
       <c r="W12" s="2" t="n">
-        <v>45267</v>
+        <v>45503</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">DANIEL ALVES SANTOS DE OLIVEIRA </t>
+          <t>SABRINA FARIAS DE ALMEIDA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>485.948.938-17</t>
+          <t>395.792.568-10</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>11-94928-7741</t>
+          <t>11-98938-5786</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">dan.alves899@gmail.com </t>
+          <t xml:space="preserve">sabrinafarias22@hotmail.com </t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>AZOR MARTIN GRILO</t>
+          <t>SANDRA D´ ANGELO  MONTENEGRO</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>082.202.578-73</t>
+          <t>163.408.318-00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>11 94498-7971</t>
+          <t>11-97503-4446</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t xml:space="preserve">azorgrilo@bol.com.br </t>
+          <t>sdmontenegro@uol.com.br</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Rua Benedito dos Santos, 464 - Jundiapeba</t>
+          <t>Rua Engenheiro Gualberto, 366 - Centro</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -1480,16 +1478,16 @@
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr">
         <is>
-          <t>1.500,00</t>
+          <t>854,00</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>06/06/2024</t>
+          <t>12/01/2023</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
@@ -1504,56 +1502,56 @@
       </c>
       <c r="U13" t="inlineStr"/>
       <c r="V13" s="2" t="n">
-        <v>45511</v>
+        <v>45262</v>
       </c>
       <c r="W13" s="2" t="n">
-        <v>45511</v>
+        <v>45119</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>VINICIUS DE MORAES TORRAGA</t>
+          <t xml:space="preserve">DANIEL ALVES SANTOS DE OLIVEIRA </t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>254.146.088-06</t>
+          <t>485.948.938-17</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11 98185-3391</t>
+          <t>11-94928-7741</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">vinlu22@hotmail.com </t>
+          <t xml:space="preserve">dan.alves899@gmail.com </t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>SANDRA D´ ANGELO  MONTENEGRO</t>
+          <t>AZOR MARTIN GRILO</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>163.408.318-00</t>
+          <t>082.202.578-73</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>11-97503-4446</t>
+          <t>11 94498-7971</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>sdmontenegro@uol.com.br</t>
+          <t xml:space="preserve">azorgrilo@bol.com.br </t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Rua Engenheiro Gualberto, 372 - Centro</t>
+          <t xml:space="preserve"> Rua Benedito dos Santos, 464 - Jundiapeba</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -1561,16 +1559,16 @@
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
         <is>
-          <t>754,00</t>
+          <t>1.500,00</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>15/03/2024</t>
+          <t>06/06/2024</t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
@@ -1585,31 +1583,31 @@
       </c>
       <c r="U14" t="inlineStr"/>
       <c r="V14" s="2" t="n">
-        <v>45397</v>
+        <v>45511</v>
       </c>
       <c r="W14" s="2" t="n">
-        <v>45488</v>
+        <v>45481</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ANDERSON ( N.A.)</t>
+          <t>VINICIUS DE MORAES TORRAGA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>364.303.858-50</t>
+          <t>254.146.088-06</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>11 97219-6319</t>
+          <t>11 98185-3391</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">starscreeamtattu@gmail.com </t>
+          <t xml:space="preserve">vinlu22@hotmail.com </t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1634,7 +1632,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Rua Engenheiro Gualberto, 358 - Centro</t>
+          <t xml:space="preserve"> Rua Engenheiro Gualberto, 372 - Centro</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
@@ -1642,12 +1640,12 @@
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>754,00</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>30/03/2024</t>
+          <t>15/03/2024</t>
         </is>
       </c>
       <c r="O15" t="n">
@@ -1666,31 +1664,31 @@
       </c>
       <c r="U15" t="inlineStr"/>
       <c r="V15" s="2" t="n">
-        <v>45412</v>
+        <v>45397</v>
       </c>
       <c r="W15" s="2" t="n">
-        <v>45503</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>FEAL ESQUADRIAS MOGI DAS CRUZES LTDA</t>
+          <t>ANDERSON ( N.A.)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>04.796.962/0001-50</t>
+          <t>364.303.858-50</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>11-97576-5544</t>
+          <t>11 97219-6319</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">feal.adm@uol.com.br </t>
+          <t xml:space="preserve">starscreeamtattu@gmail.com </t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1715,7 +1713,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Rua Cabo Diogo Oliver, 75 - Centro</t>
+          <t>Rua Engenheiro Gualberto, 358 - Centro</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
@@ -1723,16 +1721,16 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
         <is>
-          <t>7.000,00</t>
+          <t>750</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>01/02/2023</t>
+          <t>30/03/2024</t>
         </is>
       </c>
       <c r="O16" t="n">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
@@ -1747,7 +1745,7 @@
       </c>
       <c r="U16" t="inlineStr"/>
       <c r="V16" s="2" t="n">
-        <v>44985</v>
+        <v>45412</v>
       </c>
       <c r="W16" s="2" t="n">
         <v>45503</v>
@@ -1756,22 +1754,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ANTONIO CARLOS DE MATTOS GUERRA</t>
+          <t>FEAL ESQUADRIAS MOGI DAS CRUZES LTDA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>073.114.838-08</t>
+          <t>04.796.962/0001-50</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>11-91255-4242</t>
+          <t>11-97576-5544</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">mattos.guerra@uol.com.br </t>
+          <t xml:space="preserve">feal.adm@uol.com.br </t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1796,7 +1794,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Rua Engenheiro Gualberto, 362 -  Centro</t>
+          <t>Rua Cabo Diogo Oliver, 75 - Centro</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
@@ -1804,16 +1802,16 @@
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr">
         <is>
-          <t>850,00</t>
+          <t>7.000,00</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>05/04/2024</t>
+          <t>01/02/2023</t>
         </is>
       </c>
       <c r="O17" t="n">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
@@ -1828,31 +1826,31 @@
       </c>
       <c r="U17" t="inlineStr"/>
       <c r="V17" s="2" t="n">
-        <v>45417</v>
+        <v>44985</v>
       </c>
       <c r="W17" s="2" t="n">
-        <v>45419</v>
+        <v>45503</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DDP INDUSTRIA E COMERCIO LTDA</t>
+          <t>ANTONIO CARLOS DE MATTOS GUERRA</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08.267.165/0001-36</t>
+          <t>073.114.838-08</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>11-97525-2115</t>
+          <t>11-91255-4242</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">walter.e@ddp.ind.br </t>
+          <t xml:space="preserve">mattos.guerra@uol.com.br </t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1877,7 +1875,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Rua Basílio Marques, 27 - Centro</t>
+          <t>Rua Engenheiro Gualberto, 362 -  Centro</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
@@ -1885,16 +1883,16 @@
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
-          <t>3.500,00</t>
+          <t>850,00</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>05/01/2024</t>
+          <t>05/04/2024</t>
         </is>
       </c>
       <c r="O18" t="n">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
@@ -1909,31 +1907,31 @@
       </c>
       <c r="U18" t="inlineStr"/>
       <c r="V18" s="2" t="n">
-        <v>45414</v>
+        <v>45417</v>
       </c>
       <c r="W18" s="2" t="n">
-        <v>45419</v>
+        <v>45478</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ELZA PEREIRA DA SILVA</t>
+          <t>DDP INDUSTRIA E COMERCIO LTDA</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>091.155.088-70</t>
+          <t>08.267.165/0001-36</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>11-97186-6191</t>
+          <t>11-97525-2115</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">elzasilva1001@gmail.com </t>
+          <t xml:space="preserve">walter.e@ddp.ind.br </t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1958,7 +1956,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Rua Engenheiro Gualberto, 374 - Centro</t>
+          <t>Rua Basílio Marques, 27 - Centro</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -1966,16 +1964,16 @@
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr">
         <is>
-          <t>754,00</t>
+          <t>3.500,00</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>20/02/2024</t>
+          <t>05/01/2024</t>
         </is>
       </c>
       <c r="O19" t="n">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
@@ -1990,56 +1988,56 @@
       </c>
       <c r="U19" t="inlineStr"/>
       <c r="V19" s="2" t="n">
-        <v>45371</v>
+        <v>45414</v>
       </c>
       <c r="W19" s="2" t="n">
-        <v>45493</v>
+        <v>45478</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>HUMBERTO FERNANDO SOARES MAZZA</t>
+          <t>ELZA PEREIRA DA SILVA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>321.624.708-29</t>
+          <t>091.155.088-70</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>11-97400-0243</t>
+          <t>11-97186-6191</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">mazzahumberto@gmail.com </t>
+          <t xml:space="preserve">elzasilva1001@gmail.com </t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>AZOR MARTIN GRILO</t>
+          <t>SANDRA D´ ANGELO  MONTENEGRO</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>082.202.578-73</t>
+          <t>163.408.318-00</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>11 94498-7971</t>
+          <t>11-97503-4446</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t xml:space="preserve">azorgrilo@bol.com.br </t>
+          <t>sdmontenegro@uol.com.br</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Rua Benedito dos Santos, 454 - Jundiapeba</t>
+          <t>Rua Engenheiro Gualberto, 374 - Centro</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
@@ -2047,16 +2045,16 @@
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>
-          <t>1.500,00</t>
+          <t>754,00</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>04/03/2024</t>
+          <t>20/02/2024</t>
         </is>
       </c>
       <c r="O20" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
@@ -2071,31 +2069,31 @@
       </c>
       <c r="U20" t="inlineStr"/>
       <c r="V20" s="2" t="n">
-        <v>45539</v>
+        <v>45371</v>
       </c>
       <c r="W20" s="2" t="n">
-        <v>45542</v>
+        <v>45493</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ASSOCIAÇÃO BENEFICIENTE CRISTÃ CULTURAL EDUCACIONAL FRUTIFICAR - ABEF</t>
+          <t>HUMBERTO FERNANDO SOARES MAZZA</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>03.032.523/0001-08</t>
+          <t>321.624.708-29</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>11-99578-4676</t>
+          <t>11-97400-0243</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve">fernandohiraki@yahoo.com.br </t>
+          <t xml:space="preserve">mazzahumberto@gmail.com </t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2120,7 +2118,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Rua Benedito dos Santos, 684 - Jundiapeba</t>
+          <t>Rua Benedito dos Santos, 454 - Jundiapeba</t>
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
@@ -2128,16 +2126,16 @@
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr">
         <is>
-          <t>3.240,00</t>
+          <t>1.500,00</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>26/07/2023</t>
+          <t>04/03/2024</t>
         </is>
       </c>
       <c r="O21" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
@@ -2152,52 +2150,56 @@
       </c>
       <c r="U21" t="inlineStr"/>
       <c r="V21" s="2" t="n">
-        <v>45164</v>
+        <v>45539</v>
       </c>
       <c r="W21" s="2" t="n">
-        <v>45499</v>
+        <v>45482</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LUKAS SANTANA AUGUSTO</t>
+          <t>ASSOCIAÇÃO BENEFICIENTE CRISTÃ CULTURAL EDUCACIONAL FRUTIFICAR - ABEF</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>230.616.900-08</t>
+          <t>03.032.523/0001-08</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>11-99828-2203</t>
+          <t>11-99578-4676</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>adm@propagavisual.com.br</t>
+          <t xml:space="preserve">fernandohiraki@yahoo.com.br </t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>CARMEM  LOZANO GRILO</t>
+          <t>AZOR MARTIN GRILO</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>154.429.658-47</t>
+          <t>082.202.578-73</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>11 97335-7542</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
+          <t>11 94498-7971</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">azorgrilo@bol.com.br </t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Av. Maria Osório do Vale, 369 - Alto do Ipiranga</t>
+          <t>Rua Benedito dos Santos, 684 - Jundiapeba</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
@@ -2205,16 +2207,16 @@
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr">
         <is>
-          <t>2.100,00</t>
+          <t>3.240,00</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
+          <t>26/07/2023</t>
         </is>
       </c>
       <c r="O22" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
@@ -2225,15 +2227,163 @@
         </is>
       </c>
       <c r="T22" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U22" t="inlineStr"/>
       <c r="V22" s="2" t="n">
+        <v>45164</v>
+      </c>
+      <c r="W22" s="2" t="n">
+        <v>45499</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>LUKAS SANTANA AUGUSTO</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>230.616.900-08</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>11-99828-2203</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>adm@propagavisual.com.br</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>CARMEM  LOZANO GRILO</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>154.429.658-47</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>11 97335-7542</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Av. Maria Osório do Vale, 369 - Alto do Ipiranga</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>2.100,00</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>30</v>
+      </c>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="T23" t="n">
+        <v>10</v>
+      </c>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" s="2" t="n">
         <v>45417</v>
       </c>
-      <c r="W22" s="2" t="n">
-        <v>45419</v>
-      </c>
+      <c r="W23" s="2" t="n">
+        <v>45478</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>DOUGLAS LISBOA DOS SANTOS</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>229.462.728-85</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>11-94708-1361</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">douglaslissantos@gmail.com </t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>AZOR MARTIN GRILO</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>082.202.578-73</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>11 94498-7971</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">azorgrilo@bol.com.br </t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Rua Benedicto dos Santos, 488 - Jundiapeba</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>1.400,00</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>15/07/2024</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" s="2" t="n">
+        <v>45518</v>
+      </c>
+      <c r="W24" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>